<commit_message>
Fehler des static last_point behoben
Signed-off-by: Bobbbl <sebastian.draxinger@googlemail.com>
</commit_message>
<xml_diff>
--- a/Umrechnung-Koordinaten-in-Schritte.xlsx
+++ b/Umrechnung-Koordinaten-in-Schritte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F44783-4ACA-4038-AF94-24F5C81062E6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5AA985-044E-4AE2-8C43-13B45EDCDCB2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3750" xr2:uid="{D260E698-33DD-4849-826A-CDCDDB09A779}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3750" firstSheet="2" activeTab="2" xr2:uid="{D260E698-33DD-4849-826A-CDCDDB09A779}"/>
   </bookViews>
   <sheets>
     <sheet name="Koordinaten" sheetId="1" r:id="rId1"/>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94722A06-100F-4FAD-8342-7D8A783301C5}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,24 +665,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2">
         <f>E2-B2</f>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1">
         <f>B8/B5</f>
-        <v>1.4142135623730951</v>
+        <v>24.020824298928627</v>
       </c>
       <c r="M2" s="7">
         <v>400</v>
@@ -693,13 +693,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -727,7 +727,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f>SQRT(H2^2+H3^2)</f>
-        <v>1.4142135623730951</v>
+        <v>24.020824298928627</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +757,7 @@
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f>Koordinaten!H2*Koordinaten!M2</f>
-        <v>400</v>
+        <v>9600</v>
       </c>
       <c r="C3" s="1">
         <f>Koordinaten!H3*Koordinaten!M2</f>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA547B21-BB33-41B6-8D14-B893144306D2}">
   <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="D3" s="1">
         <f>'Millimeter in Schritte'!B3/Umdrehungen!A3</f>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1">
         <f>'Millimeter in Schritte'!C3/Umdrehungen!B3</f>
@@ -838,11 +838,11 @@
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f>Umdrehungen!D3/Koordinaten!K2*60</f>
-        <v>84.852813742385692</v>
+        <v>119.89596877108224</v>
       </c>
       <c r="C4" s="1">
         <f>Umdrehungen!E3/Koordinaten!K2*60</f>
-        <v>84.852813742385692</v>
+        <v>4.9956653654617602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>